<commit_message>
add column map support
</commit_message>
<xml_diff>
--- a/tools/stone-do-generator/entities.xlsx
+++ b/tools/stone-do-generator/entities.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fengxie/MyProjects/y2019/platform/stone/tools/stone-do-generator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fengxie/MyProjects/y2019/xxyhj/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BA4AD3-A924-674D-94C2-E5B04BFD2C0B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD7DBF7-D46A-BD45-AC95-A736AAB07277}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18880" tabRatio="783" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18880" tabRatio="783" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TransactionLabel" sheetId="64" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="102">
   <si>
     <t>Label</t>
   </si>
@@ -169,9 +169,6 @@
     <t>url</t>
   </si>
   <si>
-    <t>version</t>
-  </si>
-  <si>
     <t>points</t>
   </si>
   <si>
@@ -190,9 +187,6 @@
     <t>Permission</t>
   </si>
   <si>
-    <t>1:N</t>
-  </si>
-  <si>
     <t>permissionList</t>
   </si>
   <si>
@@ -247,9 +241,6 @@
     <t>积分规则</t>
   </si>
   <si>
-    <t>版本</t>
-  </si>
-  <si>
     <t>银行用户</t>
   </si>
   <si>
@@ -322,12 +313,6 @@
     <t>N:N</t>
   </si>
   <si>
-    <t>AdminRole</t>
-  </si>
-  <si>
-    <t>roles</t>
-  </si>
-  <si>
     <t>等级</t>
   </si>
   <si>
@@ -340,10 +325,22 @@
     <t>用户姓名</t>
   </si>
   <si>
-    <t>user_roles</t>
-  </si>
-  <si>
-    <t>规则备注</t>
+    <t>每金额产生积分</t>
+  </si>
+  <si>
+    <t>customized</t>
+  </si>
+  <si>
+    <t>是否可自定义积分</t>
+  </si>
+  <si>
+    <t>sequence:100</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>com.hkrt.xbank.manager.RoleCacheHolder</t>
   </si>
 </sst>
 </file>
@@ -409,7 +406,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -469,6 +466,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -480,7 +488,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -504,6 +512,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -859,7 +873,7 @@
   <dimension ref="A1:V29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:N4"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -890,7 +904,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -958,34 +972,34 @@
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>9</v>
@@ -1038,7 +1052,7 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -1054,7 +1068,7 @@
         <v>40</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1062,7 +1076,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -1076,7 +1090,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1084,7 +1098,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -1110,7 +1124,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -1206,10 +1220,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C1950AB-5D85-FE4D-AEA8-532B5EFA72D0}">
-  <dimension ref="A1:AO26"/>
+  <dimension ref="A1:AO16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -1220,7 +1234,7 @@
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
@@ -1236,7 +1250,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1330,22 +1344,22 @@
       <c r="AO2" s="3"/>
     </row>
     <row r="3" spans="1:41" ht="16">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="9"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
@@ -1385,34 +1399,34 @@
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>9</v>
@@ -1498,7 +1512,7 @@
     </row>
     <row r="6" spans="1:41" ht="16">
       <c r="A6" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>24</v>
@@ -1509,7 +1523,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -1547,7 +1561,7 @@
     </row>
     <row r="7" spans="1:41" ht="16">
       <c r="A7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>27</v>
@@ -1558,7 +1572,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -1596,18 +1610,20 @@
     </row>
     <row r="8" spans="1:41" ht="16">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="C8" s="1">
+        <v>512</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -1644,20 +1660,13 @@
       <c r="AO8" s="3"/>
     </row>
     <row r="9" spans="1:41" ht="16">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
+      <c r="A9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="9"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
@@ -1687,20 +1696,21 @@
       <c r="AO9" s="3"/>
     </row>
     <row r="10" spans="1:41" ht="16">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
@@ -1735,15 +1745,6 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
@@ -1778,15 +1779,6 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
@@ -1821,15 +1813,6 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
@@ -1864,15 +1847,6 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
@@ -1907,15 +1881,6 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
@@ -1950,15 +1915,6 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
@@ -1987,379 +1943,10 @@
       <c r="AN16" s="3"/>
       <c r="AO16" s="3"/>
     </row>
-    <row r="17" spans="1:41" ht="16">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-      <c r="S17" s="3"/>
-      <c r="T17" s="3"/>
-      <c r="U17" s="3"/>
-      <c r="V17" s="3"/>
-      <c r="W17" s="3"/>
-      <c r="X17" s="3"/>
-      <c r="Y17" s="3"/>
-      <c r="Z17" s="3"/>
-      <c r="AA17" s="3"/>
-      <c r="AB17" s="3"/>
-      <c r="AC17" s="3"/>
-      <c r="AD17" s="3"/>
-      <c r="AE17" s="3"/>
-      <c r="AF17" s="3"/>
-      <c r="AG17" s="3"/>
-      <c r="AH17" s="3"/>
-      <c r="AI17" s="3"/>
-      <c r="AJ17" s="3"/>
-      <c r="AK17" s="3"/>
-      <c r="AL17" s="3"/>
-      <c r="AM17" s="3"/>
-      <c r="AN17" s="3"/>
-      <c r="AO17" s="3"/>
-    </row>
-    <row r="18" spans="1:41" ht="16">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
-      <c r="T18" s="3"/>
-      <c r="U18" s="3"/>
-      <c r="V18" s="3"/>
-      <c r="W18" s="3"/>
-      <c r="X18" s="3"/>
-      <c r="Y18" s="3"/>
-      <c r="Z18" s="3"/>
-      <c r="AA18" s="3"/>
-      <c r="AB18" s="3"/>
-      <c r="AC18" s="3"/>
-      <c r="AD18" s="3"/>
-      <c r="AE18" s="3"/>
-      <c r="AF18" s="3"/>
-      <c r="AG18" s="3"/>
-      <c r="AH18" s="3"/>
-      <c r="AI18" s="3"/>
-      <c r="AJ18" s="3"/>
-      <c r="AK18" s="3"/>
-      <c r="AL18" s="3"/>
-      <c r="AM18" s="3"/>
-      <c r="AN18" s="3"/>
-      <c r="AO18" s="3"/>
-    </row>
-    <row r="19" spans="1:41" ht="16">
-      <c r="A19" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="9"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
-      <c r="V19" s="3"/>
-      <c r="W19" s="3"/>
-      <c r="X19" s="3"/>
-      <c r="Y19" s="3"/>
-      <c r="Z19" s="3"/>
-      <c r="AA19" s="3"/>
-      <c r="AB19" s="3"/>
-      <c r="AC19" s="3"/>
-      <c r="AD19" s="3"/>
-      <c r="AE19" s="3"/>
-      <c r="AF19" s="3"/>
-      <c r="AG19" s="3"/>
-      <c r="AH19" s="3"/>
-      <c r="AI19" s="3"/>
-      <c r="AJ19" s="3"/>
-      <c r="AK19" s="3"/>
-      <c r="AL19" s="3"/>
-      <c r="AM19" s="3"/>
-      <c r="AN19" s="3"/>
-      <c r="AO19" s="3"/>
-    </row>
-    <row r="20" spans="1:41" ht="16">
-      <c r="A20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
-      <c r="U20" s="3"/>
-      <c r="V20" s="3"/>
-      <c r="W20" s="3"/>
-      <c r="X20" s="3"/>
-      <c r="Y20" s="3"/>
-      <c r="Z20" s="3"/>
-      <c r="AA20" s="3"/>
-      <c r="AB20" s="3"/>
-      <c r="AC20" s="3"/>
-      <c r="AD20" s="3"/>
-      <c r="AE20" s="3"/>
-      <c r="AF20" s="3"/>
-      <c r="AG20" s="3"/>
-      <c r="AH20" s="3"/>
-      <c r="AI20" s="3"/>
-      <c r="AJ20" s="3"/>
-      <c r="AK20" s="3"/>
-      <c r="AL20" s="3"/>
-      <c r="AM20" s="3"/>
-      <c r="AN20" s="3"/>
-      <c r="AO20" s="3"/>
-    </row>
-    <row r="21" spans="1:41" ht="16">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
-      <c r="U21" s="3"/>
-      <c r="V21" s="3"/>
-      <c r="W21" s="3"/>
-      <c r="X21" s="3"/>
-      <c r="Y21" s="3"/>
-      <c r="Z21" s="3"/>
-      <c r="AA21" s="3"/>
-      <c r="AB21" s="3"/>
-      <c r="AC21" s="3"/>
-      <c r="AD21" s="3"/>
-      <c r="AE21" s="3"/>
-      <c r="AF21" s="3"/>
-      <c r="AG21" s="3"/>
-      <c r="AH21" s="3"/>
-      <c r="AI21" s="3"/>
-      <c r="AJ21" s="3"/>
-      <c r="AK21" s="3"/>
-      <c r="AL21" s="3"/>
-      <c r="AM21" s="3"/>
-      <c r="AN21" s="3"/>
-      <c r="AO21" s="3"/>
-    </row>
-    <row r="22" spans="1:41" ht="16">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
-      <c r="T22" s="3"/>
-      <c r="U22" s="3"/>
-      <c r="V22" s="3"/>
-      <c r="W22" s="3"/>
-      <c r="X22" s="3"/>
-      <c r="Y22" s="3"/>
-      <c r="Z22" s="3"/>
-      <c r="AA22" s="3"/>
-      <c r="AB22" s="3"/>
-      <c r="AC22" s="3"/>
-      <c r="AD22" s="3"/>
-      <c r="AE22" s="3"/>
-      <c r="AF22" s="3"/>
-      <c r="AG22" s="3"/>
-      <c r="AH22" s="3"/>
-      <c r="AI22" s="3"/>
-      <c r="AJ22" s="3"/>
-      <c r="AK22" s="3"/>
-      <c r="AL22" s="3"/>
-      <c r="AM22" s="3"/>
-      <c r="AN22" s="3"/>
-      <c r="AO22" s="3"/>
-    </row>
-    <row r="23" spans="1:41" ht="16">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
-      <c r="S23" s="3"/>
-      <c r="T23" s="3"/>
-      <c r="U23" s="3"/>
-      <c r="V23" s="3"/>
-      <c r="W23" s="3"/>
-      <c r="X23" s="3"/>
-      <c r="Y23" s="3"/>
-      <c r="Z23" s="3"/>
-      <c r="AA23" s="3"/>
-      <c r="AB23" s="3"/>
-      <c r="AC23" s="3"/>
-      <c r="AD23" s="3"/>
-      <c r="AE23" s="3"/>
-      <c r="AF23" s="3"/>
-      <c r="AG23" s="3"/>
-      <c r="AH23" s="3"/>
-      <c r="AI23" s="3"/>
-      <c r="AJ23" s="3"/>
-      <c r="AK23" s="3"/>
-      <c r="AL23" s="3"/>
-      <c r="AM23" s="3"/>
-      <c r="AN23" s="3"/>
-      <c r="AO23" s="3"/>
-    </row>
-    <row r="24" spans="1:41" ht="16">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="3"/>
-      <c r="S24" s="3"/>
-      <c r="T24" s="3"/>
-      <c r="U24" s="3"/>
-      <c r="V24" s="3"/>
-      <c r="W24" s="3"/>
-      <c r="X24" s="3"/>
-      <c r="Y24" s="3"/>
-      <c r="Z24" s="3"/>
-      <c r="AA24" s="3"/>
-      <c r="AB24" s="3"/>
-      <c r="AC24" s="3"/>
-      <c r="AD24" s="3"/>
-      <c r="AE24" s="3"/>
-      <c r="AF24" s="3"/>
-      <c r="AG24" s="3"/>
-      <c r="AH24" s="3"/>
-      <c r="AI24" s="3"/>
-      <c r="AJ24" s="3"/>
-      <c r="AK24" s="3"/>
-      <c r="AL24" s="3"/>
-      <c r="AM24" s="3"/>
-      <c r="AN24" s="3"/>
-      <c r="AO24" s="3"/>
-    </row>
-    <row r="25" spans="1:41" ht="16">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="3"/>
-      <c r="S25" s="3"/>
-      <c r="T25" s="3"/>
-      <c r="U25" s="3"/>
-      <c r="V25" s="3"/>
-      <c r="W25" s="3"/>
-      <c r="X25" s="3"/>
-      <c r="Y25" s="3"/>
-      <c r="Z25" s="3"/>
-      <c r="AA25" s="3"/>
-      <c r="AB25" s="3"/>
-      <c r="AC25" s="3"/>
-      <c r="AD25" s="3"/>
-      <c r="AE25" s="3"/>
-      <c r="AF25" s="3"/>
-      <c r="AG25" s="3"/>
-      <c r="AH25" s="3"/>
-      <c r="AI25" s="3"/>
-      <c r="AJ25" s="3"/>
-      <c r="AK25" s="3"/>
-      <c r="AL25" s="3"/>
-      <c r="AM25" s="3"/>
-      <c r="AN25" s="3"/>
-      <c r="AO25" s="3"/>
-    </row>
-    <row r="26" spans="1:41" ht="16">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="3"/>
-      <c r="R26" s="3"/>
-      <c r="S26" s="3"/>
-      <c r="T26" s="3"/>
-      <c r="U26" s="3"/>
-      <c r="V26" s="3"/>
-      <c r="W26" s="3"/>
-      <c r="X26" s="3"/>
-      <c r="Y26" s="3"/>
-      <c r="Z26" s="3"/>
-      <c r="AA26" s="3"/>
-      <c r="AB26" s="3"/>
-      <c r="AC26" s="3"/>
-      <c r="AD26" s="3"/>
-      <c r="AE26" s="3"/>
-      <c r="AF26" s="3"/>
-      <c r="AG26" s="3"/>
-      <c r="AH26" s="3"/>
-      <c r="AI26" s="3"/>
-      <c r="AJ26" s="3"/>
-      <c r="AK26" s="3"/>
-      <c r="AL26" s="3"/>
-      <c r="AM26" s="3"/>
-      <c r="AN26" s="3"/>
-      <c r="AO26" s="3"/>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A19:E19"/>
+  <mergeCells count="2">
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A3:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2398,7 +1985,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2462,34 +2049,34 @@
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>9</v>
@@ -2529,7 +2116,7 @@
     </row>
     <row r="6" spans="1:22" ht="16">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>27</v>
@@ -2541,7 +2128,7 @@
         <v>20</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -2563,7 +2150,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -2681,7 +2268,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2760,34 +2347,34 @@
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>9</v>
@@ -2832,7 +2419,7 @@
     </row>
     <row r="6" spans="1:22" ht="16">
       <c r="A6" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>21</v>
@@ -2847,7 +2434,7 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -2876,7 +2463,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -2974,21 +2561,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6A5C563-44AE-2243-A494-43FAFA5524BC}">
-  <dimension ref="A1:Z23"/>
+  <dimension ref="A1:Z9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
     <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
@@ -3004,7 +2592,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -3084,34 +2672,34 @@
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>9</v>
@@ -3144,7 +2732,9 @@
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="F5" s="1" t="s">
         <v>11</v>
       </c>
@@ -3192,335 +2782,55 @@
       <c r="R6" s="3"/>
     </row>
     <row r="7" spans="1:26" ht="16">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
+      <c r="A7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
     </row>
     <row r="8" spans="1:26" ht="16">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
     </row>
     <row r="9" spans="1:26" ht="16">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
-    </row>
-    <row r="10" spans="1:26" ht="16">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-    </row>
-    <row r="11" spans="1:26" ht="16">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-    </row>
-    <row r="12" spans="1:26" ht="16">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-    </row>
-    <row r="13" spans="1:26" ht="16">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-    </row>
-    <row r="14" spans="1:26" ht="16">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-    </row>
-    <row r="15" spans="1:26" ht="16">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
-    </row>
-    <row r="16" spans="1:26" ht="16">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-    </row>
-    <row r="17" spans="1:18" ht="16">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-    </row>
-    <row r="18" spans="1:18" ht="16">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-    </row>
-    <row r="19" spans="1:18" ht="16">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-    </row>
-    <row r="20" spans="1:18" ht="16">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-    </row>
-    <row r="21" spans="1:18" ht="16">
-      <c r="A21" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="9"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-    </row>
-    <row r="22" spans="1:18" ht="16">
-      <c r="A22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-    </row>
-    <row r="23" spans="1:18" ht="16">
-      <c r="A23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A7:E7"/>
     <mergeCell ref="A3:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3529,22 +2839,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3B3684F-4DA6-6145-A67B-9039BC61E00D}">
-  <dimension ref="A1:R14"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
     <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.83203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
@@ -3560,7 +2869,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -3636,34 +2945,34 @@
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>9</v>
@@ -3703,7 +3012,7 @@
     </row>
     <row r="6" spans="1:18" ht="16">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>23</v>
@@ -3718,7 +3027,7 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -3748,7 +3057,7 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -3776,7 +3085,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -3804,7 +3113,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -3821,7 +3130,7 @@
         <v>23</v>
       </c>
       <c r="C10" s="1">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -3830,7 +3139,7 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -3841,72 +3150,97 @@
     </row>
     <row r="11" spans="1:18" ht="16">
       <c r="A11" s="1" t="s">
-        <v>49</v>
+        <v>100</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="1">
-        <v>256</v>
-      </c>
+      <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
+      <c r="L11" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:18" ht="16">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="1">
+        <v>256</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="1:18" ht="16">
+      <c r="A13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="9"/>
-    </row>
-    <row r="13" spans="1:18" ht="16">
-      <c r="A13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:18" ht="16">
       <c r="A14" s="1" t="s">
-        <v>94</v>
+        <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>95</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D14" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="E14" s="1" t="s">
-        <v>101</v>
-      </c>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="16">
+      <c r="A15" s="11"/>
+    </row>
+    <row r="16" spans="1:18" ht="16">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+    </row>
+    <row r="17" spans="1:3" ht="16">
+      <c r="A17" s="10"/>
+    </row>
+    <row r="18" spans="1:3" ht="16">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A13:E13"/>
     <mergeCell ref="A3:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3946,7 +3280,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -4025,34 +3359,34 @@
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>9</v>
@@ -4116,7 +3450,7 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -4132,7 +3466,7 @@
     </row>
     <row r="7" spans="1:26" ht="16">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>23</v>
@@ -4147,7 +3481,7 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -4245,10 +3579,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{432A45DD-DA44-F741-89E5-B4C715FD05F9}">
-  <dimension ref="A1:Y17"/>
+  <dimension ref="A1:Y26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -4274,7 +3608,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -4356,34 +3690,34 @@
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>9</v>
@@ -4435,7 +3769,7 @@
         <v>40</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -4443,7 +3777,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -4473,7 +3807,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -4503,7 +3837,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -4531,7 +3865,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -4547,13 +3881,20 @@
       <c r="T9" s="3"/>
     </row>
     <row r="10" spans="1:25" ht="16">
-      <c r="A10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="9"/>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
@@ -4562,21 +3903,20 @@
       <c r="T10" s="3"/>
     </row>
     <row r="11" spans="1:25" ht="16">
-      <c r="A11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
@@ -4590,6 +3930,15 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
@@ -4603,6 +3952,21 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
     </row>
     <row r="14" spans="1:25" ht="16">
       <c r="A14" s="1"/>
@@ -4610,6 +3974,21 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
     </row>
     <row r="15" spans="1:25" ht="16">
       <c r="A15" s="1"/>
@@ -4617,6 +3996,21 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
     </row>
     <row r="16" spans="1:25" ht="16">
       <c r="A16" s="1"/>
@@ -4624,17 +4018,155 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" ht="16">
+      <c r="F16" s="1"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+    </row>
+    <row r="17" spans="1:20" ht="16">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+    </row>
+    <row r="18" spans="1:20" ht="16">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
+    </row>
+    <row r="19" spans="1:20" ht="16">
+      <c r="A19" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="9"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
+    </row>
+    <row r="20" spans="1:20" ht="16">
+      <c r="A20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+    </row>
+    <row r="21" spans="1:20" ht="16">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+    </row>
+    <row r="22" spans="1:20" ht="16">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:20" ht="16">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:20" ht="16">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:20" ht="16">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:20" ht="16">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A19:E19"/>
     <mergeCell ref="A3:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4646,7 +4178,7 @@
   <dimension ref="A1:AD18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -4673,7 +4205,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -4785,34 +4317,34 @@
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>9</v>
@@ -4876,7 +4408,7 @@
     </row>
     <row r="6" spans="1:30" ht="16">
       <c r="A6" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>23</v>
@@ -4891,7 +4423,7 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -4918,7 +4450,7 @@
     </row>
     <row r="7" spans="1:30" ht="16">
       <c r="A7" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>30</v>
@@ -4931,7 +4463,7 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -4958,7 +4490,7 @@
     </row>
     <row r="8" spans="1:30" ht="16">
       <c r="A8" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>23</v>
@@ -4969,7 +4501,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -5007,7 +4539,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -5045,7 +4577,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -5261,10 +4793,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{861FA028-581D-FE4C-A613-7121E26D7A7E}">
-  <dimension ref="A1:Z22"/>
+  <dimension ref="A1:Z17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -5273,7 +4805,7 @@
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="4.6640625" bestFit="1" customWidth="1"/>
@@ -5291,7 +4823,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -5386,34 +4918,34 @@
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>9</v>
@@ -5466,20 +4998,20 @@
     </row>
     <row r="6" spans="1:26" ht="16">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="1">
-        <v>32</v>
+        <v>200</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -5499,20 +5031,20 @@
     </row>
     <row r="7" spans="1:26" ht="16">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="1">
-        <v>64</v>
+        <v>512</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -5531,14 +5063,20 @@
       <c r="W7" s="3"/>
     </row>
     <row r="8" spans="1:26" ht="16">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -5556,14 +5094,20 @@
       <c r="W8" s="3"/>
     </row>
     <row r="9" spans="1:26" ht="16">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -5581,20 +5125,13 @@
       <c r="W9" s="3"/>
     </row>
     <row r="10" spans="1:26" ht="16">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
+      <c r="A10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="9"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
@@ -5606,20 +5143,21 @@
       <c r="W10" s="3"/>
     </row>
     <row r="11" spans="1:26" ht="16">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
@@ -5636,15 +5174,6 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
@@ -5661,15 +5190,6 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
@@ -5686,15 +5206,6 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
@@ -5706,13 +5217,11 @@
       <c r="W14" s="3"/>
     </row>
     <row r="15" spans="1:26" ht="16">
-      <c r="A15" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="9"/>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
@@ -5724,21 +5233,11 @@
       <c r="W15" s="3"/>
     </row>
     <row r="16" spans="1:26" ht="16">
-      <c r="A16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
@@ -5765,89 +5264,9 @@
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
     </row>
-    <row r="18" spans="1:23" ht="16">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
-      <c r="T18" s="3"/>
-      <c r="U18" s="3"/>
-      <c r="V18" s="3"/>
-      <c r="W18" s="3"/>
-    </row>
-    <row r="19" spans="1:23" ht="16">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
-      <c r="V19" s="3"/>
-      <c r="W19" s="3"/>
-    </row>
-    <row r="20" spans="1:23" ht="16">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
-      <c r="U20" s="3"/>
-      <c r="V20" s="3"/>
-      <c r="W20" s="3"/>
-    </row>
-    <row r="21" spans="1:23" ht="16">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
-      <c r="U21" s="3"/>
-      <c r="V21" s="3"/>
-      <c r="W21" s="3"/>
-    </row>
-    <row r="22" spans="1:23" ht="16">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
-      <c r="T22" s="3"/>
-      <c r="U22" s="3"/>
-      <c r="V22" s="3"/>
-      <c r="W22" s="3"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A10:E10"/>
     <mergeCell ref="A3:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
change unique index to index
</commit_message>
<xml_diff>
--- a/tools/stone-do-generator/entities.xlsx
+++ b/tools/stone-do-generator/entities.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fengxie/MyProjects/y2019/xxyhj/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fengxie/MyProjects/y2019/platform/stone/tools/stone-do-generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD7DBF7-D46A-BD45-AC95-A736AAB07277}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CDC191-B518-2545-A9FF-6AA829AEAAE5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18880" tabRatio="783" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18880" tabRatio="783" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TransactionLabel" sheetId="64" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="103">
   <si>
     <t>Label</t>
   </si>
@@ -341,6 +341,9 @@
   </si>
   <si>
     <t>com.hkrt.xbank.manager.RoleCacheHolder</t>
+  </si>
+  <si>
+    <t>bank_user</t>
   </si>
 </sst>
 </file>
@@ -504,6 +507,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -512,12 +521,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -944,22 +947,22 @@
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:22" ht="16">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="11"/>
     </row>
     <row r="4" spans="1:22" ht="16">
       <c r="A4" s="1" t="s">
@@ -1134,13 +1137,13 @@
       <c r="N9" s="1"/>
     </row>
     <row r="10" spans="1:22" ht="16">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="11"/>
     </row>
     <row r="11" spans="1:22" ht="16">
       <c r="A11" s="1" t="s">
@@ -1344,22 +1347,22 @@
       <c r="AO2" s="3"/>
     </row>
     <row r="3" spans="1:41" ht="16">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="11"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
@@ -1660,13 +1663,13 @@
       <c r="AO8" s="3"/>
     </row>
     <row r="9" spans="1:41" ht="16">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
@@ -2021,22 +2024,22 @@
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:22" ht="16">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="11"/>
     </row>
     <row r="4" spans="1:22" ht="16">
       <c r="A4" s="1" t="s">
@@ -2160,13 +2163,13 @@
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:22" ht="16">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="11"/>
     </row>
     <row r="9" spans="1:22" ht="16">
       <c r="A9" s="1" t="s">
@@ -2314,22 +2317,22 @@
       <c r="S2" s="3"/>
     </row>
     <row r="3" spans="1:22" ht="16">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="11"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
@@ -2478,13 +2481,13 @@
       <c r="S7" s="3"/>
     </row>
     <row r="8" spans="1:22" ht="16">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="11"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
@@ -2640,22 +2643,22 @@
       <c r="R2" s="3"/>
     </row>
     <row r="3" spans="1:26" ht="16">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="11"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
@@ -2782,13 +2785,13 @@
       <c r="R6" s="3"/>
     </row>
     <row r="7" spans="1:26" ht="16">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="11"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
@@ -2841,7 +2844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3B3684F-4DA6-6145-A67B-9039BC61E00D}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
@@ -2913,22 +2916,22 @@
       <c r="R2" s="3"/>
     </row>
     <row r="3" spans="1:18" ht="16">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="11"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
@@ -3197,13 +3200,13 @@
       <c r="N12" s="1"/>
     </row>
     <row r="13" spans="1:18" ht="16">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="9"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="11"/>
     </row>
     <row r="14" spans="1:18" ht="16">
       <c r="A14" s="1" t="s">
@@ -3223,20 +3226,20 @@
       </c>
     </row>
     <row r="15" spans="1:18" ht="16">
-      <c r="A15" s="11"/>
+      <c r="A15" s="8"/>
     </row>
     <row r="16" spans="1:18" ht="16">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
     </row>
     <row r="17" spans="1:3" ht="16">
-      <c r="A17" s="10"/>
+      <c r="A17" s="7"/>
     </row>
     <row r="18" spans="1:3" ht="16">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3326,22 +3329,22 @@
       <c r="S2" s="3"/>
     </row>
     <row r="3" spans="1:26" ht="16">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="11"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
@@ -3496,13 +3499,13 @@
       <c r="S7" s="3"/>
     </row>
     <row r="8" spans="1:26" ht="16">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="11"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
@@ -3656,22 +3659,22 @@
       <c r="T2" s="3"/>
     </row>
     <row r="3" spans="1:25" ht="16">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="11"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
@@ -4079,13 +4082,13 @@
       <c r="T18" s="3"/>
     </row>
     <row r="19" spans="1:20" ht="16">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="11"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
@@ -4177,8 +4180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C415122D-D6F8-444D-B6DC-E59430DC332F}">
   <dimension ref="A1:AD18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -4273,22 +4276,22 @@
       <c r="AD2" s="3"/>
     </row>
     <row r="3" spans="1:30" ht="16">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="11"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
@@ -4427,7 +4430,9 @@
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
+      <c r="K6" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -4603,13 +4608,13 @@
       <c r="AD10" s="3"/>
     </row>
     <row r="11" spans="1:30" ht="16">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="9"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="11"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
@@ -4881,22 +4886,22 @@
       <c r="W2" s="3"/>
     </row>
     <row r="3" spans="1:26" ht="16">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="11"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
@@ -5125,13 +5130,13 @@
       <c r="W9" s="3"/>
     </row>
     <row r="10" spans="1:26" ht="16">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="11"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>

</xml_diff>